<commit_message>
EPBDS: added support of user defined conditions
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/conditions/FieldMappingConditionsTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/conditions/FieldMappingConditionsTest.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C7:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -693,34 +693,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C5:C11"/>
+  <dimension ref="B5:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:3">
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="6" t="s">
+    <row r="6" spans="2:2" ht="30">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="3:3">
-      <c r="C10" s="5" t="s">
+    <row r="10" spans="2:2">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="3:3">
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="2:2" ht="30">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>